<commit_message>
listeners, screenshot and more tests for login page added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\CURSOS CARLOS\APPIUM\Proyecto\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611D139B-40C7-43D9-BF57-EA681639407A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B9EC9F-8CFA-46B2-823B-A6F68CE7E93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5276542-3268-47FC-9423-1E5177CCB985}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B5276542-3268-47FC-9423-1E5177CCB985}"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="errorInfoMessages" sheetId="2" r:id="rId2"/>
+    <sheet name="credentialsErrorMessages" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>key</t>
   </si>
@@ -78,6 +80,39 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>missingFirstName</t>
+  </si>
+  <si>
+    <t>missingLastName</t>
+  </si>
+  <si>
+    <t>missingZipCode</t>
+  </si>
+  <si>
+    <t>Error: First Name is required</t>
+  </si>
+  <si>
+    <t>Error: Last Name is required</t>
+  </si>
+  <si>
+    <t>Error: Postal Code is required</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Sorry, this user has been locked out.</t>
+  </si>
+  <si>
+    <t>Username and password do not match any user in this service.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -468,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA83E7F-0321-4CA6-9E20-4B9DD2339C6A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,4 +584,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71EC1C3-DF79-4E66-AC81-AF6A5A22B838}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D420F11D-BE11-4E40-B622-744A2670392A}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>